<commit_message>
Ingresan tareas de sprint 2 a documento Burndown Chart
</commit_message>
<xml_diff>
--- a/Documentación/Burndown Chart.xlsx
+++ b/Documentación/Burndown Chart.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebaa\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13081C1A-370E-4103-9194-6276F90689CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D260A8DD-1472-4F8D-A6C6-67BB7A356305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
-    <sheet name="Estimación de tareas" sheetId="2" r:id="rId2"/>
-    <sheet name="Matriz RACI" sheetId="3" r:id="rId3"/>
+    <sheet name="Burndown Chart Sprint2" sheetId="5" r:id="rId1"/>
+    <sheet name="Burndown Chart" sheetId="1" r:id="rId2"/>
+    <sheet name="Estimación de tareas" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="Matriz RACI" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>BURNDOWN CHART</t>
   </si>
@@ -62,9 +64,6 @@
     <t>Estimación de tareas</t>
   </si>
   <si>
-    <t>Tarea</t>
-  </si>
-  <si>
     <t>Rodrigo</t>
   </si>
   <si>
@@ -88,12 +87,75 @@
   <si>
     <t>Evaluar tareas en horas</t>
   </si>
+  <si>
+    <t>HE3</t>
+  </si>
+  <si>
+    <t>HA1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>Yo como cuidador deberé entregar datos, además de los datos de el paciente al administrador para que este me cree un perfil entregándome un nombre de usuario y clave predefinida.</t>
+  </si>
+  <si>
+    <t>HC5</t>
+  </si>
+  <si>
+    <t>Crear perfil paciente con user y password</t>
+  </si>
+  <si>
+    <t>Crear vista para actualizar datos del paciente</t>
+  </si>
+  <si>
+    <t>HC1</t>
+  </si>
+  <si>
+    <t>Yo como cuidador podré visualizar y descargar los diferentes documentos respecto al paciente para mantenerte informado sobre el diagnóstico y evolución del paciente.</t>
+  </si>
+  <si>
+    <t>Vista para acceder a documentos del repositorio</t>
+  </si>
+  <si>
+    <t>Yo como especialista en terreno tendré la opción de pedir al administrador que cambie un paciente para otro grupo o cambiarlo para otra fecha en caso de un inconveniente</t>
+  </si>
+  <si>
+    <t>Opción de contacto con el administrador con el fin de modificar la ruta</t>
+  </si>
+  <si>
+    <t>Yo como administrador de la página web podré ingresar pacientes y cuidadores, al programa de hospitalización domiciliaria, para poder tener un registro de sus datos.</t>
+  </si>
+  <si>
+    <t>Crear Login de ADM, con permisos de creacion de nuevos usuarios </t>
+  </si>
+  <si>
+    <t>Vista de cuenta administrador para realizar update o delete de informacion o perfiles usuarios</t>
+  </si>
+  <si>
+    <t>DIAS</t>
+  </si>
+  <si>
+    <t>Revisar, modificar y consolidar modelo de base de datos.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tarea ID</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +200,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -171,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,31 +247,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,6 +297,498 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CL"/>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart Sprint2'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart Sprint2'!$A$6:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A48E-4823-8033-45814F2EB032}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart Sprint2'!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planificado</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart Sprint2'!$D$6:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A48E-4823-8033-45814F2EB032}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart Sprint2'!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart Sprint2'!$E$6:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A48E-4823-8033-45814F2EB032}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="518726704"/>
+        <c:axId val="518727024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="518726704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518727024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="518727024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="518726704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -753,6 +1320,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1269,7 +1876,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{840B3A0F-6F20-4873-BD90-FFD84D0710CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1606,11 +2772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AECEA0C-FB70-45F2-823C-CAE9161CDEB9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09B837-E531-46BB-88CC-65AFFDB79DED}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,50 +2785,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
@@ -1681,191 +2847,191 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>0</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>120</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>120</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2">
         <f>C6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <f>$D$6-SUM($B$6:B6)</f>
         <v>120</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <f>IF(C7 ="",NA(),$E$6 -SUM($C$7:C7))</f>
         <v>119</v>
       </c>
-      <c r="F7" s="1">
-        <f t="shared" ref="F7:F15" si="0">C7</f>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F20" si="0">C7</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <f>$D$6-SUM($B$6:B7)</f>
         <v>120</v>
       </c>
-      <c r="E8" s="1" t="e">
+      <c r="E8" s="2" t="e">
         <f>IF(C8 ="",NA(),$E$6 -SUM($C$7:C8))</f>
         <v>#N/A</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
         <f>$D$6-SUM($B$6:B8)</f>
         <v>120</v>
       </c>
-      <c r="E9" s="1" t="e">
+      <c r="E9" s="2" t="e">
         <f>IF(C9 ="",NA(),$E$6 -SUM($C$7:C9))</f>
         <v>#N/A</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>4</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
         <f>$D$6-SUM($B$6:B9)</f>
         <v>120</v>
       </c>
-      <c r="E10" s="1" t="e">
+      <c r="E10" s="2" t="e">
         <f>IF(C10 ="",NA(),$E$6 -SUM($C$7:C10))</f>
         <v>#N/A</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>5</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <f>$D$6-SUM($B$6:B10)</f>
         <v>120</v>
       </c>
-      <c r="E11" s="1" t="e">
+      <c r="E11" s="2" t="e">
         <f>IF(C11 ="",NA(),$E$6 -SUM($C$7:C11))</f>
         <v>#N/A</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>6</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <f>$D$6-SUM($B$6:B11)</f>
         <v>120</v>
       </c>
-      <c r="E12" s="1" t="e">
+      <c r="E12" s="2" t="e">
         <f>IF(C12 ="",NA(),$E$6 -SUM($C$7:C12))</f>
         <v>#N/A</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>7</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <f>$D$6-SUM($B$6:B12)</f>
         <v>120</v>
       </c>
-      <c r="E13" s="1" t="e">
+      <c r="E13" s="2" t="e">
         <f>IF(C13 ="",NA(),$E$6 -SUM($C$7:C13))</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <f>$D$6-SUM($B$6:B13)</f>
         <v>120</v>
       </c>
-      <c r="E14" s="1" t="e">
+      <c r="E14" s="2" t="e">
         <f>IF(C14 ="",NA(),$E$6 -SUM($C$7:C14))</f>
         <v>#N/A</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>9</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <f>$D$6-SUM($B$6:B14)</f>
         <v>120</v>
       </c>
-      <c r="E15" s="1" t="e">
+      <c r="E15" s="2" t="e">
         <f>IF(C15 ="",NA(),$E$6 -SUM($C$7:C15))</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1882,11 +3048,287 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AECEA0C-FB70-45F2-823C-CAE9161CDEB9}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>120</v>
+      </c>
+      <c r="E6" s="1">
+        <v>120</v>
+      </c>
+      <c r="F6" s="1">
+        <f>C6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f>$D$6-SUM($B$6:B6)</f>
+        <v>120</v>
+      </c>
+      <c r="E7" s="1">
+        <f>IF(C7 ="",NA(),$E$6 -SUM($C$7:C7))</f>
+        <v>119</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F15" si="0">C7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <f>$D$6-SUM($B$6:B7)</f>
+        <v>120</v>
+      </c>
+      <c r="E8" s="1" t="e">
+        <f>IF(C8 ="",NA(),$E$6 -SUM($C$7:C8))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <f>$D$6-SUM($B$6:B8)</f>
+        <v>120</v>
+      </c>
+      <c r="E9" s="1" t="e">
+        <f>IF(C9 ="",NA(),$E$6 -SUM($C$7:C9))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <f>$D$6-SUM($B$6:B9)</f>
+        <v>120</v>
+      </c>
+      <c r="E10" s="1" t="e">
+        <f>IF(C10 ="",NA(),$E$6 -SUM($C$7:C10))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f>$D$6-SUM($B$6:B10)</f>
+        <v>120</v>
+      </c>
+      <c r="E11" s="1" t="e">
+        <f>IF(C11 ="",NA(),$E$6 -SUM($C$7:C11))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1">
+        <f>$D$6-SUM($B$6:B11)</f>
+        <v>120</v>
+      </c>
+      <c r="E12" s="1" t="e">
+        <f>IF(C12 ="",NA(),$E$6 -SUM($C$7:C12))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <f>$D$6-SUM($B$6:B12)</f>
+        <v>120</v>
+      </c>
+      <c r="E13" s="1" t="e">
+        <f>IF(C13 ="",NA(),$E$6 -SUM($C$7:C13))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <f>$D$6-SUM($B$6:B13)</f>
+        <v>120</v>
+      </c>
+      <c r="E14" s="1" t="e">
+        <f>IF(C14 ="",NA(),$E$6 -SUM($C$7:C14))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <f>$D$6-SUM($B$6:B14)</f>
+        <v>120</v>
+      </c>
+      <c r="E15" s="1" t="e">
+        <f>IF(C15 ="",NA(),$E$6 -SUM($C$7:C15))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4377FFF-3459-4A63-A70A-2C6B0B97F03C}">
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C22"/>
+      <selection activeCell="D5" sqref="D5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,114 +3344,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="L1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="L1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" t="e">
         <f>AVERAGE(D5:I5)</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="10">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2020,15 +3454,17 @@
         <f t="shared" ref="J6:J41" si="0">AVERAGE(D6:I6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="10">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2041,9 +3477,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="10">
+        <v>4</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2056,9 +3494,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="10">
+        <v>5</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2071,9 +3511,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2086,9 +3528,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="10">
+        <v>7</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2101,9 +3545,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2116,9 +3560,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2131,9 +3575,9 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2146,9 +3590,9 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2161,9 +3605,9 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2176,9 +3620,9 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2191,9 +3635,9 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2206,9 +3650,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2221,9 +3665,9 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2236,9 +3680,9 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2251,9 +3695,9 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2266,9 +3710,9 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2281,9 +3725,9 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2296,9 +3740,9 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2311,9 +3755,9 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2326,135 +3770,135 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="J27" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="J28" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="J29" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="J30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="J31" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="J32" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="J33" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
       <c r="J34" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="J35" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="J36" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="J37" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
       <c r="J38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
       <c r="J39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
       <c r="J40" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="J41" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2462,6 +3906,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="L1:O6"/>
@@ -2478,36 +3946,181 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6050803-4FD8-4B18-81B1-D67E91D41811}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD60ABA-6089-440F-8D9A-B0BEE075CC07}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Brundown chart, modificacion horas totales
</commit_message>
<xml_diff>
--- a/Documentación/Burndown Chart.xlsx
+++ b/Documentación/Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebaa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Segundo Semestre 2019\Software II\GITHUB\Grupo04_Hospitalizacion-Domiciliaria\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BEFA07-643A-46FE-831C-EA60B752CDE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717A8227-3EEC-4365-B972-AA4C3372D65A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Sprint2" sheetId="5" r:id="rId1"/>
@@ -270,6 +270,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -282,26 +291,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,7 +412,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -499,7 +499,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -586,7 +586,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="00B0F0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -602,13 +602,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -2842,8 +2842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09B837-E531-46BB-88CC-65AFFDB79DED}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2852,43 +2852,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="4" t="s">
         <v>3</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>56</v>
       </c>
       <c r="E6" s="2">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2">
         <f>C6</f>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="E7" s="2">
         <f>IF(C7 ="",NA(),$E$6 -SUM($C$7:C7))</f>
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" ref="F7:F20" si="0">C7</f>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="E8" s="8">
         <f>IF(C8 ="",NA(),$E$6 -SUM($C$7:C8))</f>
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
@@ -3233,7 +3233,8 @@
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3258,53 +3259,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="L1" s="16" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="L1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -3326,17 +3327,17 @@
       <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="18">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="1">
         <v>16</v>
       </c>
@@ -3357,17 +3358,17 @@
         <f>AVERAGE(D5:I5)</f>
         <v>15.2</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="18">
         <v>2</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="1">
         <v>4</v>
       </c>
@@ -3385,20 +3386,20 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J41" si="0">AVERAGE(D6:I6)</f>
+        <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:I6)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="18">
         <v>3</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="1">
         <v>8</v>
       </c>
@@ -3421,11 +3422,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="18">
         <v>4</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="1">
         <v>8</v>
       </c>
@@ -3448,11 +3449,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="18">
         <v>5</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="1">
         <v>8</v>
       </c>
@@ -3475,11 +3476,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="18">
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="1">
         <v>4</v>
       </c>
@@ -3502,11 +3503,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="18">
         <v>7</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="1">
         <v>8</v>
       </c>
@@ -3529,9 +3530,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -3540,15 +3541,15 @@
       <c r="I12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="18">
+      <c r="J12" s="11">
         <f>SUM(J5:J11)</f>
         <v>56.2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -3557,9 +3558,9 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -3568,9 +3569,9 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -3579,9 +3580,9 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -3590,9 +3591,9 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -3601,9 +3602,9 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -3612,9 +3613,9 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -3623,9 +3624,9 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3634,9 +3635,9 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -3645,9 +3646,9 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3656,9 +3657,9 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3667,9 +3668,9 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -3678,9 +3679,9 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -3689,9 +3690,9 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -3700,82 +3701,106 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="L1:O6"/>
@@ -3792,30 +3817,6 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3825,7 +3826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6050803-4FD8-4B18-81B1-D67E91D41811}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3836,65 +3837,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="14">
         <v>16</v>
       </c>
       <c r="D4" t="s">
@@ -3936,38 +3937,38 @@
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3987,38 +3988,38 @@
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -4038,38 +4039,38 @@
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -4137,43 +4138,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Update de Estimacion de tareas
Agregue mi estimacion de tareas. Cristian
</commit_message>
<xml_diff>
--- a/Documentación/Burndown Chart.xlsx
+++ b/Documentación/Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Segundo Semestre 2019\Software II\GITHUB\Grupo04_Hospitalizacion-Domiciliaria\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Desktop\Hospital\G4HD\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717A8227-3EEC-4365-B972-AA4C3372D65A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82120E02-7FD8-46F1-99CA-3AF17ADB280B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Sprint2" sheetId="5" r:id="rId1"/>
@@ -291,14 +291,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2842,16 +2842,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09B837-E531-46BB-88CC-65AFFDB79DED}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2866,7 +2866,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -2879,7 +2879,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="17" t="s">
         <v>5</v>
@@ -2893,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>2</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>4</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>5</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>6</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>7</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>8</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>9</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>10</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>11</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>12</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>13</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>14</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="8"/>
     </row>
   </sheetData>
@@ -3242,70 +3242,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4377FFF-3459-4A63-A70A-2C6B0B97F03C}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="L1" s="20" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="L1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-    </row>
-    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+    </row>
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -3327,12 +3327,12 @@
       <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>1</v>
       </c>
@@ -3344,7 +3344,9 @@
       <c r="E5" s="1">
         <v>16</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>16</v>
+      </c>
       <c r="G5" s="1">
         <v>16</v>
       </c>
@@ -3356,14 +3358,14 @@
       </c>
       <c r="J5">
         <f>AVERAGE(D5:I5)</f>
-        <v>15.2</v>
-      </c>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>15.333333333333334</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>2</v>
       </c>
@@ -3375,7 +3377,9 @@
       <c r="E6" s="1">
         <v>4</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
       <c r="G6" s="1">
         <v>4</v>
       </c>
@@ -3387,14 +3391,14 @@
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:I6)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>3</v>
       </c>
@@ -3406,7 +3410,9 @@
       <c r="E7" s="1">
         <v>7</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>8</v>
+      </c>
       <c r="G7" s="1">
         <v>8</v>
       </c>
@@ -3418,10 +3424,10 @@
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6.833333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="18">
         <v>4</v>
       </c>
@@ -3433,7 +3439,9 @@
       <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
       <c r="G8" s="1">
         <v>8</v>
       </c>
@@ -3445,10 +3453,10 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9.6666666666666661</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>5</v>
       </c>
@@ -3460,7 +3468,9 @@
       <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
       <c r="G9" s="1">
         <v>10</v>
       </c>
@@ -3472,10 +3482,10 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9.3333333333333339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>6</v>
       </c>
@@ -3487,7 +3497,9 @@
       <c r="E10" s="1">
         <v>4</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
       <c r="G10" s="1">
         <v>4</v>
       </c>
@@ -3502,7 +3514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="18">
         <v>7</v>
       </c>
@@ -3514,7 +3526,9 @@
       <c r="E11" s="1">
         <v>6</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>8</v>
+      </c>
       <c r="G11" s="1">
         <v>8</v>
       </c>
@@ -3526,10 +3540,10 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -3543,10 +3557,10 @@
       </c>
       <c r="J12" s="11">
         <f>SUM(J5:J11)</f>
-        <v>56.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>56.833333333333336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -3557,7 +3571,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -3568,7 +3582,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -3579,7 +3593,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -3590,7 +3604,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -3601,7 +3615,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -3612,7 +3626,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -3623,7 +3637,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -3634,7 +3648,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -3645,7 +3659,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -3656,7 +3670,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -3667,7 +3681,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -3678,7 +3692,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -3689,7 +3703,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -3700,107 +3714,83 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="L1:O6"/>
@@ -3817,6 +3807,30 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3830,13 +3844,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
@@ -3857,7 +3871,7 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="13"/>
       <c r="C2" s="12" t="s">
@@ -3876,7 +3890,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -3891,7 +3905,7 @@
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3905,7 +3919,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3919,7 +3933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3933,10 +3947,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="13"/>
       <c r="C8" s="12" t="s">
@@ -3955,7 +3969,7 @@
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3970,7 +3984,7 @@
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3984,10 +3998,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="12" t="s">
@@ -4006,7 +4020,7 @@
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
     </row>
-    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="12"/>
@@ -4021,7 +4035,7 @@
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
     </row>
-    <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>5</v>
       </c>
@@ -4035,10 +4049,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="12" t="s">
@@ -4057,7 +4071,7 @@
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="12"/>
@@ -4072,7 +4086,7 @@
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>6</v>
       </c>
@@ -4086,7 +4100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>7</v>
       </c>
@@ -4118,7 +4132,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4132,12 +4146,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4152,7 +4166,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -4165,7 +4179,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="17" t="s">
         <v>5</v>
@@ -4179,7 +4193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -4199,7 +4213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -4216,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -4237,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -4256,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -4275,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -4294,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -4313,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -4332,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -4351,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -4370,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
burndown Chart actualizado - Sebastian Herrera
</commit_message>
<xml_diff>
--- a/Documentación/Burndown Chart.xlsx
+++ b/Documentación/Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebaa\Grupo04_Hospitalizacion-Domiciliaria\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6D5AE8-86F0-4332-AB0F-441341CAF94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248509F-935E-4A9A-9C75-5946264E6BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
+    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Sprint2" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>BURNDOWN CHART</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Evaluar tareas en horas</t>
   </si>
   <si>
-    <t>HE3</t>
-  </si>
-  <si>
     <t>HA1</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>HC5</t>
   </si>
   <si>
-    <t>Crear perfil paciente con user y password</t>
-  </si>
-  <si>
     <t>Crear vista para actualizar datos del paciente</t>
   </si>
   <si>
@@ -106,12 +100,6 @@
     <t>Vista para acceder a documentos del repositorio</t>
   </si>
   <si>
-    <t>Yo como especialista en terreno tendré la opción de pedir al administrador que cambie un paciente para otro grupo o cambiarlo para otra fecha en caso de un inconveniente</t>
-  </si>
-  <si>
-    <t>Opción de contacto con el administrador con el fin de modificar la ruta</t>
-  </si>
-  <si>
     <t>Yo como administrador de la página web podré ingresar pacientes y cuidadores, al programa de hospitalización domiciliaria, para poder tener un registro de sus datos.</t>
   </si>
   <si>
@@ -145,9 +133,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>T3</t>
-  </si>
-  <si>
     <t>HC1.2</t>
   </si>
   <si>
@@ -169,12 +154,6 @@
     <t>Vista Documentos</t>
   </si>
   <si>
-    <t>HE3.1</t>
-  </si>
-  <si>
-    <t>Contacto al hospital</t>
-  </si>
-  <si>
     <t>HA1.1</t>
   </si>
   <si>
@@ -209,6 +188,15 @@
   </si>
   <si>
     <t>Día de término</t>
+  </si>
+  <si>
+    <t>Fecha inicio</t>
+  </si>
+  <si>
+    <t>fecha termino</t>
+  </si>
+  <si>
+    <t>Día de término Real</t>
   </si>
 </sst>
 </file>
@@ -305,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +337,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -361,21 +358,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +495,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint2'!$B$6:$B$23</c:f>
+              <c:f>'Burndown Chart Sprint2'!$B$6:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>131</c:v>
                 </c:pt>
@@ -532,30 +527,48 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="15">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="16">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="17">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -602,27 +615,81 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart Sprint2'!$C$6:$C$23</c:f>
+              <c:f>'Burndown Chart Sprint2'!$C$6:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>186</c:v>
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1565,15 +1632,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
+      <xdr:colOff>47624</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1898,49 +1965,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09B837-E531-46BB-88CC-65AFFDB79DED}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -1948,14 +2015,14 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="21"/>
+      <c r="B4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>2</v>
@@ -1963,15 +2030,15 @@
       <c r="C5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1982,10 +2049,10 @@
         <v>131</v>
       </c>
       <c r="C6">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="18">
         <v>42</v>
@@ -2002,10 +2069,10 @@
         <v>131</v>
       </c>
       <c r="C7">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="18">
         <v>55</v>
@@ -2022,16 +2089,16 @@
         <v>131</v>
       </c>
       <c r="C8">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="18">
         <v>34</v>
       </c>
       <c r="G8" s="18">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2042,7 +2109,7 @@
         <v>131</v>
       </c>
       <c r="C9">
-        <v>186</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2053,7 +2120,7 @@
         <v>131</v>
       </c>
       <c r="C10">
-        <v>186</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2064,7 +2131,13 @@
         <v>131</v>
       </c>
       <c r="C11">
-        <v>186</v>
+        <v>131</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="30">
+        <v>43751</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2074,6 +2147,15 @@
       <c r="B12">
         <v>131</v>
       </c>
+      <c r="C12">
+        <v>131</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="30">
+        <v>43775</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
@@ -2082,6 +2164,9 @@
       <c r="B13">
         <v>131</v>
       </c>
+      <c r="C13">
+        <v>131</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18">
@@ -2090,14 +2175,37 @@
       <c r="B14">
         <v>131</v>
       </c>
+      <c r="C14">
+        <v>131</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>9</v>
       </c>
       <c r="B15">
-        <f>131-42</f>
-        <v>89</v>
+        <v>131</v>
+      </c>
+      <c r="C15">
+        <v>131</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="20">
+        <v>42</v>
+      </c>
+      <c r="G15" s="20">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2105,72 +2213,185 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16" si="0">131-42</f>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="C16">
+        <v>131</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20">
+        <v>55</v>
+      </c>
+      <c r="G16" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>11</v>
       </c>
       <c r="B17">
+        <v>131</v>
+      </c>
+      <c r="C17">
+        <v>131</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="20">
+        <v>34</v>
+      </c>
+      <c r="G17" s="20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>131</v>
+      </c>
+      <c r="C18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>131</v>
+      </c>
+      <c r="C19">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>14</v>
+      </c>
+      <c r="B20">
         <f>131-42</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>12</v>
-      </c>
-      <c r="B18">
+      <c r="C20">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21" si="0">131-42</f>
+        <v>89</v>
+      </c>
+      <c r="C21">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>16</v>
+      </c>
+      <c r="B22">
         <f>131-42</f>
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>13</v>
-      </c>
-      <c r="B19">
+      <c r="C22">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <f>131-42</f>
+        <v>89</v>
+      </c>
+      <c r="C23">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>89</v>
+      </c>
+      <c r="C24">
+        <f>131-42-34</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>19</v>
+      </c>
+      <c r="B25">
         <f>89-34</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <f t="shared" ref="B20:B22" si="1">89-34</f>
+      <c r="C25">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
-        <v>15</v>
-      </c>
-      <c r="B21">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:B28" si="1">89-34</f>
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>21</v>
+      </c>
+      <c r="B27">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
-        <v>16</v>
-      </c>
-      <c r="B22">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
+        <v>22</v>
+      </c>
+      <c r="B28">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
-        <v>17</v>
-      </c>
-      <c r="B23">
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
+        <v>23</v>
+      </c>
+      <c r="B29">
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2188,7 +2409,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,53 +2425,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="L1" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="L1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="A4" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2272,17 +2493,17 @@
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="25">
         <v>1</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="1">
         <v>16</v>
       </c>
@@ -2305,17 +2526,17 @@
         <f>AVERAGE(D5:I5)</f>
         <v>15.333333333333334</v>
       </c>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="25">
         <v>2</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="1">
         <v>4</v>
       </c>
@@ -2338,17 +2559,17 @@
         <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:I6)</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="25">
         <v>3</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="1">
         <v>8</v>
       </c>
@@ -2373,11 +2594,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="25">
         <v>4</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="1">
         <v>8</v>
       </c>
@@ -2402,11 +2623,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="25">
         <v>5</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="1">
         <v>8</v>
       </c>
@@ -2431,11 +2652,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="25">
         <v>6</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="1">
         <v>4</v>
       </c>
@@ -2460,11 +2681,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="25">
         <v>7</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="1">
         <v>8</v>
       </c>
@@ -2489,9 +2710,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="14"/>
@@ -2506,9 +2727,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2517,9 +2738,9 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2528,9 +2749,9 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2539,9 +2760,9 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2550,9 +2771,9 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2561,9 +2782,9 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2572,9 +2793,9 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2583,9 +2804,9 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2594,9 +2815,9 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2605,9 +2826,9 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2616,9 +2837,9 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2627,9 +2848,9 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2638,9 +2859,9 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2649,9 +2870,9 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2660,82 +2881,106 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="L1:O6"/>
@@ -2752,30 +2997,6 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2783,10 +3004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8125A6C4-2A46-4712-9487-F232D3963423}">
-  <dimension ref="A2:N64"/>
+  <dimension ref="A2:N62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,10 +3059,10 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2850,7 +3071,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -2860,10 +3081,10 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2871,7 +3092,7 @@
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -2882,10 +3103,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -2895,7 +3116,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -2904,10 +3125,10 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -2919,17 +3140,17 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -2937,21 +3158,21 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -2959,22 +3180,17 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
+      <c r="K8" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -2983,20 +3199,27 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
-      <c r="K9" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="13">
+        <f>SUM(D13,D14,D15)</f>
+        <v>131</v>
+      </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>14</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -3006,21 +3229,12 @@
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="13">
-        <f>SUM(8+26+21+34+55+55)</f>
-        <v>199</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13">
-        <v>14</v>
-      </c>
+      <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -3045,9 +3259,19 @@
       <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="13">
+        <f>C10/G10</f>
+        <v>9.3571428571428577</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="13">
+        <v>42</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -3060,18 +3284,12 @@
       <c r="N13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="13">
-        <f>C11/G11</f>
-        <v>14.214285714285714</v>
-      </c>
+      <c r="B14" s="13"/>
       <c r="C14" s="13" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D14" s="13">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -3087,10 +3305,10 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="13"/>
       <c r="C15" s="13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D15" s="13">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -3105,12 +3323,8 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="13"/>
-      <c r="C16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="13">
-        <v>55</v>
-      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -3124,12 +3338,8 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="13"/>
-      <c r="C17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="13">
-        <v>34</v>
-      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -3217,34 +3427,32 @@
       <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
@@ -3778,34 +3986,6 @@
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3813,10 +3993,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6050803-4FD8-4B18-81B1-D67E91D41811}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3827,20 +4007,20 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="C1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
@@ -3850,35 +4030,35 @@
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+        <v>18</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3886,202 +4066,140 @@
       </c>
       <c r="B4" s="11"/>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+    </row>
+    <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2"/>
       <c r="D14" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-    </row>
-    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-    </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="C1:I1"/>
     <mergeCell ref="D2:M3"/>
-    <mergeCell ref="D8:M9"/>
-    <mergeCell ref="D12:M13"/>
-    <mergeCell ref="D16:M17"/>
+    <mergeCell ref="D7:M8"/>
+    <mergeCell ref="D11:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4091,7 +4209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD60ABA-6089-440F-8D9A-B0BEE075CC07}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Presentación Semana  06-11 - Sebastián Herrera
</commit_message>
<xml_diff>
--- a/Documentación/Burndown Chart.xlsx
+++ b/Documentación/Burndown Chart.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebaa\Grupo04_Hospitalizacion-Domiciliaria\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248509F-935E-4A9A-9C75-5946264E6BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CED92A0-0E98-46C4-878D-C490A83F6007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
+    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" xr2:uid="{17DC4F56-A7E1-4C6B-A7C0-3119ACDEE41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart Sprint2" sheetId="5" r:id="rId1"/>
     <sheet name="Estimación de Horas" sheetId="2" r:id="rId2"/>
     <sheet name="Poker estimación" sheetId="6" r:id="rId3"/>
-    <sheet name="Tareas" sheetId="4" r:id="rId4"/>
-    <sheet name="Matriz RACI" sheetId="3" r:id="rId5"/>
+    <sheet name="Poker estimación completo" sheetId="7" r:id="rId4"/>
+    <sheet name="Tareas" sheetId="4" r:id="rId5"/>
+    <sheet name="Matriz RACI" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>BURNDOWN CHART</t>
   </si>
@@ -197,13 +198,79 @@
   </si>
   <si>
     <t>Día de término Real</t>
+  </si>
+  <si>
+    <t>TC 01-01</t>
+  </si>
+  <si>
+    <t>TC 01-02</t>
+  </si>
+  <si>
+    <t>TC 02-01</t>
+  </si>
+  <si>
+    <t>TC 03-01</t>
+  </si>
+  <si>
+    <t>TC 04-01</t>
+  </si>
+  <si>
+    <t>TE 04-01</t>
+  </si>
+  <si>
+    <t>TC 05-01</t>
+  </si>
+  <si>
+    <t>TE 01-01</t>
+  </si>
+  <si>
+    <t>TE 02-01</t>
+  </si>
+  <si>
+    <t>TE03-01</t>
+  </si>
+  <si>
+    <t>TE 05-01</t>
+  </si>
+  <si>
+    <t>TA 01-01</t>
+  </si>
+  <si>
+    <t>TA 01-02</t>
+  </si>
+  <si>
+    <t>TA 03-02</t>
+  </si>
+  <si>
+    <t>TA 02-01</t>
+  </si>
+  <si>
+    <t>TA 04-01</t>
+  </si>
+  <si>
+    <t>TA04-02</t>
+  </si>
+  <si>
+    <t>TA 05-01</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>SPRINT 2</t>
+  </si>
+  <si>
+    <t>SPRINT 1</t>
+  </si>
+  <si>
+    <t>SPRINT 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,8 +321,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +353,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -293,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,6 +437,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -358,19 +456,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,73 +604,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="15">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="16">
                   <c:v>131</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>89</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>89</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>89</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>55</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>55</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>55</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -620,73 +724,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>131</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>131</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>55</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>55</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1967,8 +2071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E09B837-E531-46BB-88CC-65AFFDB79DED}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,36 +2082,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -2015,10 +2119,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2046,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C6">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>18</v>
@@ -2058,7 +2162,7 @@
         <v>42</v>
       </c>
       <c r="G6" s="18">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2066,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C7">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>16</v>
@@ -2086,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C8">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>12</v>
@@ -2106,10 +2210,19 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C9">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="23">
+        <v>21</v>
+      </c>
+      <c r="G9" s="23">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2117,10 +2230,19 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C10">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="23">
+        <v>21</v>
+      </c>
+      <c r="G10" s="23">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2128,33 +2250,22 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C11">
-        <v>131</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="30">
-        <v>43751</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>6</v>
       </c>
       <c r="B12">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C12">
-        <v>131</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="30">
-        <v>43775</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2162,10 +2273,10 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C13">
-        <v>131</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2173,19 +2284,10 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C14">
-        <v>131</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>53</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2193,19 +2295,16 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C15">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="20">
-        <v>42</v>
-      </c>
-      <c r="G15" s="20">
-        <v>17</v>
+        <v>51</v>
+      </c>
+      <c r="F15" s="24">
+        <v>43751</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2213,19 +2312,16 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C16">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="20">
-        <v>55</v>
-      </c>
-      <c r="G16" s="20">
-        <v>17</v>
+        <v>52</v>
+      </c>
+      <c r="F16" s="24">
+        <v>43775</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,19 +2329,10 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C17">
-        <v>131</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="20">
-        <v>34</v>
-      </c>
-      <c r="G17" s="20">
-        <v>20</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,10 +2340,19 @@
         <v>12</v>
       </c>
       <c r="B18">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C18">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2264,10 +2360,19 @@
         <v>13</v>
       </c>
       <c r="B19">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="C19">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="20">
+        <v>42</v>
+      </c>
+      <c r="G19" s="20">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2275,11 +2380,20 @@
         <v>14</v>
       </c>
       <c r="B20">
-        <f>131-42</f>
-        <v>89</v>
+        <f>173-42</f>
+        <v>131</v>
       </c>
       <c r="C20">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="20">
+        <v>55</v>
+      </c>
+      <c r="G20" s="20">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2287,11 +2401,20 @@
         <v>15</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21" si="0">131-42</f>
-        <v>89</v>
+        <f>173-42</f>
+        <v>131</v>
       </c>
       <c r="C21">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="20">
+        <v>34</v>
+      </c>
+      <c r="G21" s="20">
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,11 +2422,20 @@
         <v>16</v>
       </c>
       <c r="B22">
-        <f>131-42</f>
-        <v>89</v>
+        <f t="shared" ref="B22" si="0">173-42</f>
+        <v>131</v>
       </c>
       <c r="C22">
-        <v>131</v>
+        <v>173</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="23">
+        <v>21</v>
+      </c>
+      <c r="G22" s="23">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2311,11 +2443,21 @@
         <v>17</v>
       </c>
       <c r="B23">
-        <f>131-42</f>
-        <v>89</v>
+        <f>131-55-34</f>
+        <v>42</v>
       </c>
       <c r="C23">
-        <v>131</v>
+        <f>173-42-55</f>
+        <v>76</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="23">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,11 +2465,12 @@
         <v>18</v>
       </c>
       <c r="B24">
-        <v>89</v>
+        <f t="shared" ref="B24:B28" si="1">131-55-34</f>
+        <v>42</v>
       </c>
       <c r="C24">
-        <f>131-42-34</f>
-        <v>55</v>
+        <f t="shared" ref="C24:C28" si="2">173-42-55</f>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2335,11 +2478,12 @@
         <v>19</v>
       </c>
       <c r="B25">
-        <f>89-34</f>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C25">
-        <v>55</v>
+        <f t="shared" si="2"/>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2347,11 +2491,12 @@
         <v>20</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B28" si="1">89-34</f>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C26">
-        <v>55</v>
+        <f>76-34</f>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2360,10 +2505,11 @@
       </c>
       <c r="B27">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <f t="shared" ref="C27:C28" si="3">76-34</f>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2372,10 +2518,11 @@
       </c>
       <c r="B28">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,53 +2572,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="L1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2493,17 +2640,17 @@
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="1">
         <v>16</v>
       </c>
@@ -2526,17 +2673,17 @@
         <f>AVERAGE(D5:I5)</f>
         <v>15.333333333333334</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6" s="28">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="1">
         <v>4</v>
       </c>
@@ -2559,17 +2706,17 @@
         <f t="shared" ref="J6:J11" si="0">AVERAGE(D6:I6)</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="28">
         <v>3</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="1">
         <v>8</v>
       </c>
@@ -2594,11 +2741,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="28">
         <v>4</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="1">
         <v>8</v>
       </c>
@@ -2623,11 +2770,11 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="28">
         <v>5</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="1">
         <v>8</v>
       </c>
@@ -2652,11 +2799,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="28">
         <v>6</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="1">
         <v>4</v>
       </c>
@@ -2681,11 +2828,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="A11" s="28">
         <v>7</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="1">
         <v>8</v>
       </c>
@@ -2710,9 +2857,9 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="14"/>
@@ -2727,9 +2874,9 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2738,9 +2885,9 @@
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2749,9 +2896,9 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2760,9 +2907,9 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2771,9 +2918,9 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2782,9 +2929,9 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2793,9 +2940,9 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2804,9 +2951,9 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2815,9 +2962,9 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2826,9 +2973,9 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2837,9 +2984,9 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2848,9 +2995,9 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2859,9 +3006,9 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2870,9 +3017,9 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2881,106 +3028,82 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="L1:O6"/>
@@ -2997,6 +3120,30 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3007,7 +3154,7 @@
   <dimension ref="A2:N62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A2" sqref="A2:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3992,11 +4139,237 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189EE520-DAAB-4EB0-923D-6B3CD02FE0F9}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="22">
+        <v>0</v>
+      </c>
+      <c r="D1" s="22">
+        <v>1</v>
+      </c>
+      <c r="E1" s="22">
+        <v>2</v>
+      </c>
+      <c r="F1" s="22">
+        <v>3</v>
+      </c>
+      <c r="G1" s="22">
+        <v>5</v>
+      </c>
+      <c r="H1" s="22">
+        <v>8</v>
+      </c>
+      <c r="I1" s="22">
+        <v>13</v>
+      </c>
+      <c r="J1" s="22">
+        <v>21</v>
+      </c>
+      <c r="K1" s="22">
+        <v>34</v>
+      </c>
+      <c r="L1" s="22">
+        <v>55</v>
+      </c>
+      <c r="M1" s="22">
+        <v>89</v>
+      </c>
+      <c r="N1" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="L5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="35"/>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6050803-4FD8-4B18-81B1-D67E91D41811}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,15 +4385,15 @@
       <c r="B1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
@@ -4032,33 +4405,33 @@
       <c r="C2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -4093,33 +4466,33 @@
       <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -4142,33 +4515,33 @@
       <c r="C11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
     </row>
     <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
     </row>
     <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -4205,11 +4578,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD60ABA-6089-440F-8D9A-B0BEE075CC07}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>